<commit_message>
Updated pca code (mostly colors)
Added folder with select species PCA plots
</commit_message>
<xml_diff>
--- a/pca.xlsx
+++ b/pca.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wd\rcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ppham\Documents\R\wd\rcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A79E53-8CFE-4162-842F-D1AB0674A1C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pca.pre" sheetId="4" r:id="rId1"/>
@@ -200,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -451,7 +452,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L471"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18364,7 +18365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L656"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -43305,10 +43306,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -56696,11 +56697,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L222"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -57560,8 +57561,8 @@
       <c r="F23">
         <v>43</v>
       </c>
-      <c r="G23" t="e">
-        <v>#VALUE!</v>
+      <c r="G23">
+        <v>1</v>
       </c>
       <c r="H23" t="s">
         <v>19</v>

</xml_diff>